<commit_message>
Tryna upload this ontu vercer
</commit_message>
<xml_diff>
--- a/src/excel/UsersData.xlsx
+++ b/src/excel/UsersData.xlsx
@@ -520,16 +520,16 @@
         <v>15</v>
       </c>
       <c r="G2" s="2">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="H2" s="2">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J2" s="2">
-        <v>153</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -555,13 +555,13 @@
         <v>93</v>
       </c>
       <c r="H3" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="2">
         <v>37</v>
       </c>
       <c r="J3" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>